<commit_message>
Correction of perc value
</commit_message>
<xml_diff>
--- a/data/saf_blend.xlsx
+++ b/data/saf_blend.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oburdash\dev\repos\standard_inputs\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bmfernan\dev\repos\standard_inputs\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{336D98B4-BA21-407B-B324-27F477FAC6E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EC6CCDB-B498-4773-8FA8-1D9DF460F58E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -367,7 +367,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -489,7 +489,7 @@
         <v>2030</v>
       </c>
       <c r="B9">
-        <v>0.01</v>
+        <v>0.1</v>
       </c>
       <c r="C9">
         <v>0.05</v>
@@ -509,7 +509,7 @@
         <v>0.2</v>
       </c>
       <c r="D10">
-        <v>1.6E-2</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>